<commit_message>
hotfix-dropzone by prioritizing ports
</commit_message>
<xml_diff>
--- a/front-end/input/example1card.xlsx
+++ b/front-end/input/example1card.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danni\OneDrive\מסמכים\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danni\source\repos\MemoryCards\test\MemoryCards\front-end\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DD961C3-4DA8-487F-94F6-E3115A8857D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAAA174-D535-4C66-92ED-9587054DF968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8895" yWindow="6375" windowWidth="24585" windowHeight="13440" xr2:uid="{F9F7E55B-6084-438A-B6B0-D0D9AF79A29B}"/>
+    <workbookView xWindow="11790" yWindow="7365" windowWidth="24585" windowHeight="13440" xr2:uid="{F9F7E55B-6084-438A-B6B0-D0D9AF79A29B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>2+1</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>9+1</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>front</t>
   </si>
 </sst>
 </file>
@@ -425,14 +431,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C46D676-DF54-47CA-9C8A-921A2A7A3971}">
-  <dimension ref="A2:B8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>

</xml_diff>